<commit_message>
I0 and IF added
</commit_message>
<xml_diff>
--- a/data/save_data/2021/abad_fernando.xlsx
+++ b/data/save_data/2021/abad_fernando.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>IP</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>I0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>IF</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -497,6 +507,12 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -525,6 +541,12 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -553,6 +575,12 @@
       <c r="H4" t="n">
         <v>2</v>
       </c>
+      <c r="I4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -580,6 +608,12 @@
       </c>
       <c r="H5" t="n">
         <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -609,6 +643,12 @@
       <c r="H6" t="n">
         <v>1</v>
       </c>
+      <c r="I6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -637,6 +677,12 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
+      <c r="I7" t="n">
+        <v>7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -664,6 +710,12 @@
       </c>
       <c r="H8" t="n">
         <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -693,6 +745,12 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
+      <c r="I9" t="n">
+        <v>9</v>
+      </c>
+      <c r="J9" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -721,6 +779,12 @@
       <c r="H10" t="n">
         <v>1</v>
       </c>
+      <c r="I10" t="n">
+        <v>6</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -749,6 +813,12 @@
       <c r="H11" t="n">
         <v>3</v>
       </c>
+      <c r="I11" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -777,6 +847,12 @@
       <c r="H12" t="n">
         <v>2</v>
       </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -805,6 +881,12 @@
       <c r="H13" t="n">
         <v>1</v>
       </c>
+      <c r="I13" t="n">
+        <v>9</v>
+      </c>
+      <c r="J13" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -833,6 +915,12 @@
       <c r="H14" t="n">
         <v>4</v>
       </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -861,6 +949,12 @@
       <c r="H15" t="n">
         <v>2</v>
       </c>
+      <c r="I15" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -889,6 +983,12 @@
       <c r="H16" t="n">
         <v>2</v>
       </c>
+      <c r="I16" t="n">
+        <v>7</v>
+      </c>
+      <c r="J16" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -917,6 +1017,12 @@
       <c r="H17" t="n">
         <v>1</v>
       </c>
+      <c r="I17" t="n">
+        <v>6</v>
+      </c>
+      <c r="J17" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -945,6 +1051,12 @@
       <c r="H18" t="n">
         <v>1</v>
       </c>
+      <c r="I18" t="n">
+        <v>8</v>
+      </c>
+      <c r="J18" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -973,6 +1085,12 @@
       <c r="H19" t="n">
         <v>1</v>
       </c>
+      <c r="I19" t="n">
+        <v>4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1001,6 +1119,12 @@
       <c r="H20" t="n">
         <v>1</v>
       </c>
+      <c r="I20" t="n">
+        <v>6</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1029,6 +1153,12 @@
       <c r="H21" t="n">
         <v>1</v>
       </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1057,6 +1187,12 @@
       <c r="H22" t="n">
         <v>1</v>
       </c>
+      <c r="I22" t="n">
+        <v>5</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1084,6 +1220,12 @@
       </c>
       <c r="H23" t="n">
         <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J23" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>